<commit_message>
Almost done with this analysis
</commit_message>
<xml_diff>
--- a/raw-data/testing_data.xlsx
+++ b/raw-data/testing_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gabe/Desktop/Projects/NewFinalProject/datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gabe/Desktop/Projects/Gov94Analysis/raw-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0549C407-8333-404A-BA65-9F5031F4567A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{54428D3C-577C-8F45-9B3E-8C99BE990727}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{67CCEDAB-36CE-6946-B063-650B0FE874F4}"/>
   </bookViews>
@@ -590,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21C4BAE-0AEF-1043-B97B-9F25815D16B5}">
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2106,6 +2106,12 @@
       <c r="J45">
         <v>0.8</v>
       </c>
+      <c r="K45">
+        <v>200</v>
+      </c>
+      <c r="L45">
+        <v>31</v>
+      </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">

</xml_diff>